<commit_message>
Break line longer than 256 characters
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE77BD3-C867-4BAC-B521-BF28F553CF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175B867-5825-4B51-8E37-52B4CC216FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="138">
   <si>
     <t>type</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>kl_code_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a very long note. It is longer than 256*2 characters to test what happens if a line is broken into 3 lines. Each line should only hold values up to 256 and then break line after a comma. When the line is so long that it is split into &gt;=3 lines, the second line starts with no keywords, but just list values. The last line will do the same but has to end with a semi-colon to show that the list of values has ended. With this final sentence, that had to be extended a bit, this line is now 534 characters which is long enough. </t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,7 +956,9 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Break lines longer than 256 characters (#116)
Close #113
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE77BD3-C867-4BAC-B521-BF28F553CF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175B867-5825-4B51-8E37-52B4CC216FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="138">
   <si>
     <t>type</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>kl_code_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a very long note. It is longer than 256*2 characters to test what happens if a line is broken into 3 lines. Each line should only hold values up to 256 and then break line after a comma. When the line is so long that it is split into &gt;=3 lines, the second line starts with no keywords, but just list values. The last line will do the same but has to end with a semi-colon to show that the list of values has ended. With this final sentence, that had to be extended a bit, this line is now 534 characters which is long enough. </t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,7 +956,9 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Rename figures variable. Test fails.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175B867-5825-4B51-8E37-52B4CC216FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6DB4A-CCF1-479A-86A1-EE08EA168852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="16995" windowHeight="31785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -518,9 +518,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,9 +558,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,26 +593,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,26 +628,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1188,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1258,7 +1224,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Preserve name of FIGURES variable through all data formats
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\My Drive\new\repo\pxmake\tests\testthat\fixtures\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175B867-5825-4B51-8E37-52B4CC216FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6DB4A-CCF1-479A-86A1-EE08EA168852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="16995" windowHeight="31785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -518,9 +518,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,9 +558,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,26 +593,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,26 +628,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1188,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1258,7 +1224,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Use variable-code as variable-label if no label is given
Close #173
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA3A4FF-C02E-4C56-BDEF-13C8402EFF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DC5825-EAAB-417D-A8EB-F72B8C8419E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="17025" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40275" yWindow="0" windowWidth="17325" windowHeight="16050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
   <si>
     <t>keyword</t>
   </si>
@@ -314,12 +314,6 @@
   </si>
   <si>
     <t>FIGURES</t>
-  </si>
-  <si>
-    <t>antal</t>
-  </si>
-  <si>
-    <t>amerlassusaat</t>
   </si>
   <si>
     <t>sortorder</t>
@@ -794,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1100,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,15 +1271,6 @@
       </c>
       <c r="C5" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1324,19 +1309,19 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1344,7 +1329,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1364,19 +1349,19 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
         <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1384,19 +1369,19 @@
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
         <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,7 +1389,7 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1424,19 +1409,19 @@
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
         <v>114</v>
-      </c>
-      <c r="E6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,19 +1429,19 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
         <v>118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>